<commit_message>
added sample generation and inference
</commit_message>
<xml_diff>
--- a/Inference.xlsx
+++ b/Inference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satya/Desktop/take-home/FontClassifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6B53A6-CE1F-3D4F-B035-F202C64BBFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B43EB3D-FB6B-6742-A79F-AA37ADB6BCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35240" yWindow="1500" windowWidth="28040" windowHeight="16360" xr2:uid="{1A14DA37-EDBB-AB49-82F2-7E0EC164BAED}"/>
+    <workbookView xWindow="-28040" yWindow="1480" windowWidth="28040" windowHeight="16360" xr2:uid="{1A14DA37-EDBB-AB49-82F2-7E0EC164BAED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>CPU</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>3.74s</t>
+  </si>
+  <si>
+    <t>Parameters</t>
   </si>
 </sst>
 </file>
@@ -497,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDE1EC8-6642-234D-BBB4-D2180D8DCF06}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,13 +532,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -543,13 +546,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -557,13 +560,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>0.86</v>
+        <v>0.85060000000000002</v>
       </c>
       <c r="D4" s="3">
-        <v>0.8619</v>
+        <v>0.85440000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -571,7 +574,15 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>1507706</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -579,13 +590,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -593,13 +604,13 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -607,13 +618,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
-        <v>0.85060000000000002</v>
+        <v>0.87649999999999995</v>
       </c>
       <c r="D10" s="3">
-        <v>0.85440000000000005</v>
+        <v>0.88090000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -621,7 +632,15 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>821130</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -629,13 +648,13 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -643,13 +662,13 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -657,13 +676,13 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
-        <v>0.87649999999999995</v>
+        <v>0.86</v>
       </c>
       <c r="D16" s="3">
-        <v>0.88090000000000002</v>
+        <v>0.8619</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -671,7 +690,15 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>11181642</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -713,6 +740,14 @@
       </c>
       <c r="B23" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>85806346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>